<commit_message>
fixed Hebrew WG items
</commit_message>
<xml_diff>
--- a/raw_data/Hebrew_WG/[Hebrew_WG].xlsx
+++ b/raw_data/Hebrew_WG/[Hebrew_WG].xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-7180" yWindow="-21600" windowWidth="19200" windowHeight="21160" tabRatio="500"/>
+    <workbookView xWindow="4500" yWindow="1740" windowWidth="19200" windowHeight="21160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3799" uniqueCount="1606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3803" uniqueCount="1607">
   <si>
     <t>לא לזוז</t>
   </si>
@@ -4837,6 +4837,9 @@
   </si>
   <si>
     <t>action_words</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -5274,8 +5277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J547"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A348" workbookViewId="0">
-      <selection activeCell="D386" sqref="D386"/>
+    <sheetView tabSelected="1" topLeftCell="A515" workbookViewId="0">
+      <selection activeCell="B544" sqref="B544"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5323,7 +5326,9 @@
       <c r="A2" s="1" t="s">
         <v>547</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>1606</v>
+      </c>
       <c r="C2" s="1" t="s">
         <v>1090</v>
       </c>
@@ -5339,7 +5344,9 @@
       <c r="A3" s="1" t="s">
         <v>548</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>1606</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>1090</v>
       </c>
@@ -5355,7 +5362,9 @@
       <c r="A4" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>1606</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>1090</v>
       </c>
@@ -5372,7 +5381,7 @@
         <v>550</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>0</v>
+        <v>1606</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>1091</v>
@@ -5395,7 +5404,7 @@
         <v>551</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1</v>
+        <v>1606</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>1091</v>
@@ -5418,7 +5427,7 @@
         <v>552</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>2</v>
+        <v>1606</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>1091</v>
@@ -5441,7 +5450,7 @@
         <v>553</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>3</v>
+        <v>1606</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>1091</v>
@@ -5464,7 +5473,7 @@
         <v>554</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>4</v>
+        <v>1606</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>1091</v>
@@ -5487,7 +5496,7 @@
         <v>555</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>5</v>
+        <v>1606</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>1091</v>
@@ -5510,7 +5519,7 @@
         <v>556</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>6</v>
+        <v>1606</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>1091</v>
@@ -5533,7 +5542,7 @@
         <v>557</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>7</v>
+        <v>1606</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>1091</v>
@@ -5556,7 +5565,7 @@
         <v>558</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>8</v>
+        <v>1606</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>1091</v>
@@ -5579,7 +5588,7 @@
         <v>559</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>9</v>
+        <v>1606</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>1091</v>
@@ -5602,7 +5611,7 @@
         <v>560</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>10</v>
+        <v>1606</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>1091</v>
@@ -5625,7 +5634,7 @@
         <v>561</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>11</v>
+        <v>1606</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>1091</v>
@@ -5648,7 +5657,7 @@
         <v>562</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>12</v>
+        <v>1606</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>1091</v>
@@ -5671,7 +5680,7 @@
         <v>563</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>13</v>
+        <v>1606</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>1091</v>
@@ -5694,7 +5703,7 @@
         <v>564</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>14</v>
+        <v>1606</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>1091</v>
@@ -5717,7 +5726,7 @@
         <v>565</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>15</v>
+        <v>1606</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>1091</v>
@@ -5740,7 +5749,7 @@
         <v>566</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>16</v>
+        <v>1606</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>1091</v>
@@ -5763,7 +5772,7 @@
         <v>567</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>17</v>
+        <v>1606</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>1091</v>
@@ -5786,7 +5795,7 @@
         <v>568</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>18</v>
+        <v>1606</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>1091</v>
@@ -5809,7 +5818,7 @@
         <v>569</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>19</v>
+        <v>1606</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>1091</v>
@@ -5832,7 +5841,7 @@
         <v>570</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>20</v>
+        <v>1606</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>1091</v>
@@ -5855,7 +5864,7 @@
         <v>571</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>21</v>
+        <v>1606</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>1091</v>
@@ -5878,7 +5887,7 @@
         <v>572</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>22</v>
+        <v>1606</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>1091</v>
@@ -5901,7 +5910,7 @@
         <v>573</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>23</v>
+        <v>1606</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>1091</v>
@@ -5924,7 +5933,7 @@
         <v>574</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>24</v>
+        <v>1606</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>1091</v>
@@ -5947,7 +5956,7 @@
         <v>575</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>25</v>
+        <v>1606</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>1091</v>
@@ -5970,7 +5979,7 @@
         <v>576</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>26</v>
+        <v>1606</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>527</v>
@@ -5993,7 +6002,7 @@
         <v>577</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>27</v>
+        <v>1606</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>527</v>
@@ -6016,7 +6025,7 @@
         <v>578</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>28</v>
+        <v>1606</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>527</v>
@@ -6039,7 +6048,7 @@
         <v>579</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>29</v>
+        <v>1606</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>527</v>
@@ -6062,7 +6071,7 @@
         <v>580</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>30</v>
+        <v>1606</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>527</v>
@@ -6085,7 +6094,7 @@
         <v>581</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>31</v>
+        <v>1606</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>527</v>
@@ -6108,7 +6117,7 @@
         <v>582</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>32</v>
+        <v>1606</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>527</v>
@@ -6131,7 +6140,7 @@
         <v>583</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>33</v>
+        <v>1606</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>527</v>
@@ -6154,7 +6163,7 @@
         <v>584</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>34</v>
+        <v>1606</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>527</v>
@@ -6177,7 +6186,7 @@
         <v>585</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>35</v>
+        <v>1606</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>527</v>
@@ -6200,7 +6209,7 @@
         <v>586</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>36</v>
+        <v>1606</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>527</v>
@@ -6223,7 +6232,7 @@
         <v>587</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>37</v>
+        <v>1606</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>527</v>
@@ -6246,7 +6255,7 @@
         <v>588</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>38</v>
+        <v>1606</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>527</v>
@@ -6269,7 +6278,7 @@
         <v>589</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>39</v>
+        <v>1606</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>527</v>
@@ -6292,7 +6301,7 @@
         <v>590</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>40</v>
+        <v>1606</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>527</v>
@@ -6315,7 +6324,7 @@
         <v>591</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>41</v>
+        <v>1606</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>527</v>
@@ -6338,7 +6347,7 @@
         <v>592</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>42</v>
+        <v>1606</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>527</v>
@@ -6361,7 +6370,7 @@
         <v>593</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>43</v>
+        <v>1606</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>527</v>
@@ -6384,7 +6393,7 @@
         <v>594</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>44</v>
+        <v>1606</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>527</v>
@@ -6407,7 +6416,7 @@
         <v>595</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>45</v>
+        <v>1606</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>527</v>
@@ -6430,7 +6439,7 @@
         <v>596</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>46</v>
+        <v>1606</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>527</v>
@@ -6453,7 +6462,7 @@
         <v>597</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>47</v>
+        <v>1606</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>527</v>
@@ -6476,7 +6485,7 @@
         <v>598</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>48</v>
+        <v>1606</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>527</v>
@@ -6499,7 +6508,7 @@
         <v>599</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>49</v>
+        <v>1606</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>527</v>
@@ -6522,7 +6531,7 @@
         <v>600</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>50</v>
+        <v>1606</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>527</v>
@@ -6545,7 +6554,7 @@
         <v>601</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>51</v>
+        <v>1606</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>527</v>
@@ -6568,7 +6577,7 @@
         <v>602</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>52</v>
+        <v>1606</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>527</v>
@@ -6591,7 +6600,7 @@
         <v>603</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>53</v>
+        <v>1606</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>527</v>
@@ -6614,7 +6623,7 @@
         <v>604</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>54</v>
+        <v>1606</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>527</v>
@@ -6637,7 +6646,7 @@
         <v>605</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>55</v>
+        <v>1606</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>527</v>
@@ -6660,7 +6669,7 @@
         <v>606</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>56</v>
+        <v>1606</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>527</v>
@@ -6683,7 +6692,7 @@
         <v>607</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>57</v>
+        <v>1606</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>527</v>
@@ -6706,7 +6715,7 @@
         <v>608</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>58</v>
+        <v>1606</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>527</v>
@@ -6729,7 +6738,7 @@
         <v>609</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>59</v>
+        <v>1606</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>527</v>
@@ -6752,7 +6761,7 @@
         <v>610</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>60</v>
+        <v>1606</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>527</v>
@@ -6775,7 +6784,7 @@
         <v>611</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>61</v>
+        <v>1606</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>527</v>
@@ -6798,7 +6807,7 @@
         <v>612</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>62</v>
+        <v>1606</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>527</v>
@@ -6821,7 +6830,7 @@
         <v>613</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>63</v>
+        <v>1606</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>527</v>
@@ -6844,7 +6853,7 @@
         <v>614</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>64</v>
+        <v>1606</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>527</v>
@@ -6867,7 +6876,7 @@
         <v>615</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>65</v>
+        <v>1606</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>527</v>
@@ -6890,7 +6899,7 @@
         <v>616</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>66</v>
+        <v>1606</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>527</v>
@@ -6913,7 +6922,7 @@
         <v>617</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>67</v>
+        <v>1606</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>527</v>
@@ -6936,7 +6945,7 @@
         <v>618</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>68</v>
+        <v>1606</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>527</v>
@@ -6959,7 +6968,7 @@
         <v>619</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>69</v>
+        <v>1606</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>527</v>
@@ -6982,7 +6991,7 @@
         <v>620</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>70</v>
+        <v>1606</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>527</v>
@@ -7005,7 +7014,7 @@
         <v>621</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>71</v>
+        <v>1606</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>527</v>
@@ -7028,7 +7037,7 @@
         <v>622</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>72</v>
+        <v>1606</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>527</v>
@@ -7051,7 +7060,7 @@
         <v>623</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>73</v>
+        <v>1606</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>527</v>
@@ -7074,7 +7083,7 @@
         <v>624</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>74</v>
+        <v>1606</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>527</v>
@@ -7097,7 +7106,7 @@
         <v>625</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>75</v>
+        <v>1606</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>527</v>
@@ -7120,7 +7129,7 @@
         <v>626</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>76</v>
+        <v>1606</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>527</v>
@@ -7143,7 +7152,7 @@
         <v>627</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>77</v>
+        <v>1606</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>527</v>
@@ -7166,7 +7175,7 @@
         <v>628</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>78</v>
+        <v>1606</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>527</v>
@@ -7189,7 +7198,7 @@
         <v>629</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>79</v>
+        <v>1606</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>527</v>
@@ -7212,7 +7221,7 @@
         <v>630</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>80</v>
+        <v>1606</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>527</v>
@@ -7235,7 +7244,7 @@
         <v>631</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>81</v>
+        <v>1606</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>527</v>
@@ -7258,7 +7267,7 @@
         <v>632</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>82</v>
+        <v>1606</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>527</v>
@@ -7281,7 +7290,7 @@
         <v>633</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>83</v>
+        <v>1606</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>527</v>
@@ -7304,7 +7313,7 @@
         <v>634</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>84</v>
+        <v>1606</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>527</v>
@@ -7327,7 +7336,7 @@
         <v>635</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>85</v>
+        <v>1606</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>527</v>
@@ -7350,7 +7359,7 @@
         <v>636</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>86</v>
+        <v>1606</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>527</v>
@@ -7373,7 +7382,7 @@
         <v>637</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>87</v>
+        <v>1606</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>527</v>
@@ -7396,7 +7405,7 @@
         <v>638</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>88</v>
+        <v>1606</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>527</v>
@@ -7419,7 +7428,7 @@
         <v>639</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>89</v>
+        <v>1606</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>527</v>
@@ -7442,7 +7451,7 @@
         <v>640</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>90</v>
+        <v>1606</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>527</v>
@@ -7465,7 +7474,7 @@
         <v>641</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>91</v>
+        <v>1606</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>527</v>
@@ -7488,7 +7497,7 @@
         <v>642</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>92</v>
+        <v>1606</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>527</v>
@@ -7511,7 +7520,7 @@
         <v>643</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>93</v>
+        <v>1606</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>527</v>
@@ -7534,7 +7543,7 @@
         <v>644</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>94</v>
+        <v>1606</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>527</v>
@@ -7557,7 +7566,7 @@
         <v>645</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>95</v>
+        <v>1606</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>527</v>
@@ -7580,7 +7589,7 @@
         <v>646</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>96</v>
+        <v>1606</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>527</v>
@@ -7603,7 +7612,7 @@
         <v>647</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>97</v>
+        <v>1606</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>527</v>
@@ -7626,7 +7635,7 @@
         <v>648</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>98</v>
+        <v>1606</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>527</v>
@@ -7649,7 +7658,7 @@
         <v>649</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>99</v>
+        <v>1606</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>527</v>
@@ -7672,7 +7681,7 @@
         <v>650</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>100</v>
+        <v>1606</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>527</v>
@@ -7695,7 +7704,7 @@
         <v>651</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>101</v>
+        <v>1606</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>527</v>
@@ -7718,7 +7727,7 @@
         <v>652</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>102</v>
+        <v>1606</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>527</v>
@@ -7741,7 +7750,7 @@
         <v>653</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>103</v>
+        <v>1606</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>527</v>
@@ -7764,7 +7773,7 @@
         <v>654</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>104</v>
+        <v>1606</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>527</v>
@@ -7787,7 +7796,7 @@
         <v>655</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>105</v>
+        <v>1606</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>527</v>
@@ -7810,7 +7819,7 @@
         <v>656</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>106</v>
+        <v>1606</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>527</v>
@@ -7833,7 +7842,7 @@
         <v>657</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>107</v>
+        <v>1606</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>527</v>
@@ -7856,7 +7865,7 @@
         <v>658</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>108</v>
+        <v>1606</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>527</v>
@@ -7879,7 +7888,7 @@
         <v>659</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>109</v>
+        <v>1606</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>527</v>
@@ -7902,7 +7911,7 @@
         <v>660</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>110</v>
+        <v>1606</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>527</v>
@@ -7925,7 +7934,7 @@
         <v>661</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>111</v>
+        <v>1606</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>527</v>
@@ -7948,7 +7957,7 @@
         <v>662</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>112</v>
+        <v>1606</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>527</v>
@@ -7971,7 +7980,7 @@
         <v>663</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>113</v>
+        <v>1606</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>527</v>
@@ -7994,7 +8003,7 @@
         <v>664</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>114</v>
+        <v>1606</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>527</v>
@@ -8017,7 +8026,7 @@
         <v>665</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>115</v>
+        <v>1606</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>527</v>
@@ -8040,7 +8049,7 @@
         <v>666</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>116</v>
+        <v>1606</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>527</v>
@@ -8063,7 +8072,7 @@
         <v>667</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>117</v>
+        <v>1606</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>527</v>
@@ -8086,7 +8095,7 @@
         <v>668</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>118</v>
+        <v>1606</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>527</v>
@@ -8109,7 +8118,7 @@
         <v>669</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>119</v>
+        <v>1606</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>527</v>
@@ -8132,7 +8141,7 @@
         <v>670</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>120</v>
+        <v>1606</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>527</v>
@@ -8155,7 +8164,7 @@
         <v>671</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>121</v>
+        <v>1606</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>527</v>
@@ -8178,7 +8187,7 @@
         <v>672</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>122</v>
+        <v>1606</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>527</v>
@@ -8201,7 +8210,7 @@
         <v>673</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>123</v>
+        <v>1606</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>527</v>
@@ -8224,7 +8233,7 @@
         <v>674</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>124</v>
+        <v>1606</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>527</v>
@@ -8247,7 +8256,7 @@
         <v>675</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>125</v>
+        <v>1606</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>527</v>
@@ -8270,7 +8279,7 @@
         <v>676</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>126</v>
+        <v>1606</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>527</v>
@@ -8293,7 +8302,7 @@
         <v>677</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>127</v>
+        <v>1606</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>527</v>
@@ -8316,7 +8325,7 @@
         <v>678</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>128</v>
+        <v>1606</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>527</v>
@@ -8339,7 +8348,7 @@
         <v>679</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>129</v>
+        <v>1606</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>527</v>
@@ -8362,7 +8371,7 @@
         <v>680</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>130</v>
+        <v>1606</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>527</v>
@@ -8385,7 +8394,7 @@
         <v>681</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>131</v>
+        <v>1606</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>527</v>
@@ -8408,7 +8417,7 @@
         <v>682</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>132</v>
+        <v>1606</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>527</v>
@@ -8431,7 +8440,7 @@
         <v>683</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>133</v>
+        <v>1606</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>527</v>
@@ -8454,7 +8463,7 @@
         <v>684</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>134</v>
+        <v>1606</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>527</v>
@@ -8477,7 +8486,7 @@
         <v>685</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>135</v>
+        <v>1606</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>527</v>
@@ -8500,7 +8509,7 @@
         <v>686</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>136</v>
+        <v>1606</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>527</v>
@@ -8523,7 +8532,7 @@
         <v>687</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>49</v>
+        <v>1606</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>527</v>
@@ -8546,7 +8555,7 @@
         <v>688</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>137</v>
+        <v>1606</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>527</v>
@@ -8569,7 +8578,7 @@
         <v>689</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>138</v>
+        <v>1606</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>527</v>
@@ -8592,7 +8601,7 @@
         <v>690</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>139</v>
+        <v>1606</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>527</v>
@@ -8615,7 +8624,7 @@
         <v>691</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>140</v>
+        <v>1606</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>527</v>
@@ -8638,7 +8647,7 @@
         <v>692</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>141</v>
+        <v>1606</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>527</v>
@@ -8661,7 +8670,7 @@
         <v>693</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>142</v>
+        <v>1606</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>527</v>
@@ -8684,7 +8693,7 @@
         <v>694</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>143</v>
+        <v>1606</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>527</v>
@@ -8707,7 +8716,7 @@
         <v>695</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>144</v>
+        <v>1606</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>527</v>
@@ -8730,7 +8739,7 @@
         <v>696</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>145</v>
+        <v>1606</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>527</v>
@@ -8753,7 +8762,7 @@
         <v>697</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>146</v>
+        <v>1606</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>527</v>
@@ -8776,7 +8785,7 @@
         <v>698</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>147</v>
+        <v>1606</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>527</v>
@@ -8799,7 +8808,7 @@
         <v>699</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>148</v>
+        <v>1606</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>527</v>
@@ -8822,7 +8831,7 @@
         <v>700</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>149</v>
+        <v>1606</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>527</v>
@@ -8845,7 +8854,7 @@
         <v>701</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>150</v>
+        <v>1606</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>527</v>
@@ -8868,7 +8877,7 @@
         <v>702</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>151</v>
+        <v>1606</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>527</v>
@@ -8891,7 +8900,7 @@
         <v>703</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>152</v>
+        <v>1606</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>527</v>
@@ -8914,7 +8923,7 @@
         <v>704</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>153</v>
+        <v>1606</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>527</v>
@@ -8937,7 +8946,7 @@
         <v>705</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>154</v>
+        <v>1606</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>527</v>
@@ -8960,7 +8969,7 @@
         <v>706</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>155</v>
+        <v>1606</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>527</v>
@@ -8983,7 +8992,7 @@
         <v>707</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>156</v>
+        <v>1606</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>527</v>
@@ -9006,7 +9015,7 @@
         <v>708</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>157</v>
+        <v>1606</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>527</v>
@@ -9029,7 +9038,7 @@
         <v>709</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>158</v>
+        <v>1606</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>527</v>
@@ -9052,7 +9061,7 @@
         <v>710</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>159</v>
+        <v>1606</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>527</v>
@@ -9075,7 +9084,7 @@
         <v>711</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>160</v>
+        <v>1606</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>527</v>
@@ -9098,7 +9107,7 @@
         <v>712</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>161</v>
+        <v>1606</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>527</v>
@@ -9121,7 +9130,7 @@
         <v>713</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>162</v>
+        <v>1606</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>527</v>
@@ -9144,7 +9153,7 @@
         <v>714</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>163</v>
+        <v>1606</v>
       </c>
       <c r="C169" s="1" t="s">
         <v>527</v>
@@ -9167,7 +9176,7 @@
         <v>715</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>164</v>
+        <v>1606</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>527</v>
@@ -9190,7 +9199,7 @@
         <v>716</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>165</v>
+        <v>1606</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>527</v>
@@ -9213,7 +9222,7 @@
         <v>717</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>166</v>
+        <v>1606</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>527</v>
@@ -9236,7 +9245,7 @@
         <v>718</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>167</v>
+        <v>1606</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>527</v>
@@ -9259,7 +9268,7 @@
         <v>719</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>168</v>
+        <v>1606</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>527</v>
@@ -9282,7 +9291,7 @@
         <v>720</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>169</v>
+        <v>1606</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>527</v>
@@ -9305,7 +9314,7 @@
         <v>721</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>170</v>
+        <v>1606</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>527</v>
@@ -9328,7 +9337,7 @@
         <v>722</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>171</v>
+        <v>1606</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>527</v>
@@ -9351,7 +9360,7 @@
         <v>723</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>172</v>
+        <v>1606</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>527</v>
@@ -9374,7 +9383,7 @@
         <v>724</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>173</v>
+        <v>1606</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>527</v>
@@ -9397,7 +9406,7 @@
         <v>725</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>174</v>
+        <v>1606</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>527</v>
@@ -9420,7 +9429,7 @@
         <v>726</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>175</v>
+        <v>1606</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>527</v>
@@ -9443,7 +9452,7 @@
         <v>727</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>176</v>
+        <v>1606</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>527</v>
@@ -9466,7 +9475,7 @@
         <v>728</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>177</v>
+        <v>1606</v>
       </c>
       <c r="C183" s="1" t="s">
         <v>527</v>
@@ -9489,7 +9498,7 @@
         <v>729</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>178</v>
+        <v>1606</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>527</v>
@@ -9512,7 +9521,7 @@
         <v>730</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>179</v>
+        <v>1606</v>
       </c>
       <c r="C185" s="1" t="s">
         <v>527</v>
@@ -9535,7 +9544,7 @@
         <v>731</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>180</v>
+        <v>1606</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>527</v>
@@ -9558,7 +9567,7 @@
         <v>732</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>181</v>
+        <v>1606</v>
       </c>
       <c r="C187" s="1" t="s">
         <v>527</v>
@@ -9581,7 +9590,7 @@
         <v>733</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>182</v>
+        <v>1606</v>
       </c>
       <c r="C188" s="1" t="s">
         <v>527</v>
@@ -9604,7 +9613,7 @@
         <v>734</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>183</v>
+        <v>1606</v>
       </c>
       <c r="C189" s="1" t="s">
         <v>527</v>
@@ -9627,7 +9636,7 @@
         <v>735</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>184</v>
+        <v>1606</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>527</v>
@@ -9650,7 +9659,7 @@
         <v>736</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>185</v>
+        <v>1606</v>
       </c>
       <c r="C191" s="1" t="s">
         <v>527</v>
@@ -9673,7 +9682,7 @@
         <v>737</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>186</v>
+        <v>1606</v>
       </c>
       <c r="C192" s="1" t="s">
         <v>527</v>
@@ -9696,7 +9705,7 @@
         <v>738</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>187</v>
+        <v>1606</v>
       </c>
       <c r="C193" s="1" t="s">
         <v>527</v>
@@ -9719,7 +9728,7 @@
         <v>739</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>188</v>
+        <v>1606</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>527</v>
@@ -9742,7 +9751,7 @@
         <v>740</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>189</v>
+        <v>1606</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>527</v>
@@ -9765,7 +9774,7 @@
         <v>741</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>190</v>
+        <v>1606</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>527</v>
@@ -9788,7 +9797,7 @@
         <v>742</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>191</v>
+        <v>1606</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>527</v>
@@ -9811,7 +9820,7 @@
         <v>743</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>192</v>
+        <v>1606</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>527</v>
@@ -9834,7 +9843,7 @@
         <v>744</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>193</v>
+        <v>1606</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>527</v>
@@ -9857,7 +9866,7 @@
         <v>745</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>194</v>
+        <v>1606</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>527</v>
@@ -9880,7 +9889,7 @@
         <v>746</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>195</v>
+        <v>1606</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>527</v>
@@ -9903,7 +9912,7 @@
         <v>747</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>196</v>
+        <v>1606</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>527</v>
@@ -9926,7 +9935,7 @@
         <v>748</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>197</v>
+        <v>1606</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>527</v>
@@ -9949,7 +9958,7 @@
         <v>749</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>198</v>
+        <v>1606</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>527</v>
@@ -9972,7 +9981,7 @@
         <v>750</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>199</v>
+        <v>1606</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>527</v>
@@ -9995,7 +10004,7 @@
         <v>751</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>200</v>
+        <v>1606</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>527</v>
@@ -10018,7 +10027,7 @@
         <v>752</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>201</v>
+        <v>1606</v>
       </c>
       <c r="C207" s="1" t="s">
         <v>527</v>
@@ -10041,7 +10050,7 @@
         <v>753</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>202</v>
+        <v>1606</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>527</v>
@@ -10064,7 +10073,7 @@
         <v>754</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>203</v>
+        <v>1606</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>527</v>
@@ -10087,7 +10096,7 @@
         <v>755</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>204</v>
+        <v>1606</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>527</v>
@@ -10110,7 +10119,7 @@
         <v>756</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>205</v>
+        <v>1606</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>527</v>
@@ -10133,7 +10142,7 @@
         <v>757</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>206</v>
+        <v>1606</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>527</v>
@@ -10156,7 +10165,7 @@
         <v>758</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>207</v>
+        <v>1606</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>527</v>
@@ -10179,7 +10188,7 @@
         <v>759</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>208</v>
+        <v>1606</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>527</v>
@@ -10202,7 +10211,7 @@
         <v>760</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>209</v>
+        <v>1606</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>527</v>
@@ -10225,7 +10234,7 @@
         <v>761</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>210</v>
+        <v>1606</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>527</v>
@@ -10248,7 +10257,7 @@
         <v>762</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>211</v>
+        <v>1606</v>
       </c>
       <c r="C217" s="1" t="s">
         <v>527</v>
@@ -10271,7 +10280,7 @@
         <v>763</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>212</v>
+        <v>1606</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>527</v>
@@ -10294,7 +10303,7 @@
         <v>764</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>213</v>
+        <v>1606</v>
       </c>
       <c r="C219" s="1" t="s">
         <v>527</v>
@@ -10317,7 +10326,7 @@
         <v>765</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>214</v>
+        <v>1606</v>
       </c>
       <c r="C220" s="1" t="s">
         <v>527</v>
@@ -10340,7 +10349,7 @@
         <v>766</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>215</v>
+        <v>1606</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>527</v>
@@ -10363,7 +10372,7 @@
         <v>767</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>216</v>
+        <v>1606</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>527</v>
@@ -10386,7 +10395,7 @@
         <v>768</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>217</v>
+        <v>1606</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>527</v>
@@ -10409,7 +10418,7 @@
         <v>769</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>218</v>
+        <v>1606</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>527</v>
@@ -10432,7 +10441,7 @@
         <v>770</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>219</v>
+        <v>1606</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>527</v>
@@ -10455,7 +10464,7 @@
         <v>771</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>220</v>
+        <v>1606</v>
       </c>
       <c r="C226" s="1" t="s">
         <v>527</v>
@@ -10478,7 +10487,7 @@
         <v>772</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>221</v>
+        <v>1606</v>
       </c>
       <c r="C227" s="1" t="s">
         <v>527</v>
@@ -10501,7 +10510,7 @@
         <v>773</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>222</v>
+        <v>1606</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>527</v>
@@ -10524,7 +10533,7 @@
         <v>774</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>223</v>
+        <v>1606</v>
       </c>
       <c r="C229" s="1" t="s">
         <v>527</v>
@@ -10547,7 +10556,7 @@
         <v>775</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>224</v>
+        <v>1606</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>527</v>
@@ -10570,7 +10579,7 @@
         <v>776</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>225</v>
+        <v>1606</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>527</v>
@@ -10593,7 +10602,7 @@
         <v>777</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>226</v>
+        <v>1606</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>527</v>
@@ -10616,7 +10625,7 @@
         <v>778</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>227</v>
+        <v>1606</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>527</v>
@@ -10639,7 +10648,7 @@
         <v>779</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>228</v>
+        <v>1606</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>527</v>
@@ -10662,7 +10671,7 @@
         <v>780</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>229</v>
+        <v>1606</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>527</v>
@@ -10685,7 +10694,7 @@
         <v>781</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>230</v>
+        <v>1606</v>
       </c>
       <c r="C236" s="1" t="s">
         <v>527</v>
@@ -10708,7 +10717,7 @@
         <v>782</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>231</v>
+        <v>1606</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>527</v>
@@ -10731,7 +10740,7 @@
         <v>783</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>232</v>
+        <v>1606</v>
       </c>
       <c r="C238" s="1" t="s">
         <v>527</v>
@@ -10754,7 +10763,7 @@
         <v>784</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>233</v>
+        <v>1606</v>
       </c>
       <c r="C239" s="1" t="s">
         <v>527</v>
@@ -10777,7 +10786,7 @@
         <v>785</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>234</v>
+        <v>1606</v>
       </c>
       <c r="C240" s="1" t="s">
         <v>527</v>
@@ -10800,7 +10809,7 @@
         <v>786</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>235</v>
+        <v>1606</v>
       </c>
       <c r="C241" s="1" t="s">
         <v>527</v>
@@ -10823,7 +10832,7 @@
         <v>787</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>236</v>
+        <v>1606</v>
       </c>
       <c r="C242" s="1" t="s">
         <v>527</v>
@@ -10846,7 +10855,7 @@
         <v>788</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>237</v>
+        <v>1606</v>
       </c>
       <c r="C243" s="1" t="s">
         <v>527</v>
@@ -10869,7 +10878,7 @@
         <v>789</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>238</v>
+        <v>1606</v>
       </c>
       <c r="C244" s="1" t="s">
         <v>527</v>
@@ -10892,7 +10901,7 @@
         <v>790</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>239</v>
+        <v>1606</v>
       </c>
       <c r="C245" s="1" t="s">
         <v>527</v>
@@ -10915,7 +10924,7 @@
         <v>791</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>240</v>
+        <v>1606</v>
       </c>
       <c r="C246" s="1" t="s">
         <v>527</v>
@@ -10938,7 +10947,7 @@
         <v>792</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>211</v>
+        <v>1606</v>
       </c>
       <c r="C247" s="1" t="s">
         <v>527</v>
@@ -10961,7 +10970,7 @@
         <v>793</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>241</v>
+        <v>1606</v>
       </c>
       <c r="C248" s="1" t="s">
         <v>527</v>
@@ -10984,7 +10993,7 @@
         <v>794</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>242</v>
+        <v>1606</v>
       </c>
       <c r="C249" s="1" t="s">
         <v>527</v>
@@ -11007,7 +11016,7 @@
         <v>795</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>243</v>
+        <v>1606</v>
       </c>
       <c r="C250" s="1" t="s">
         <v>527</v>
@@ -11030,7 +11039,7 @@
         <v>796</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>244</v>
+        <v>1606</v>
       </c>
       <c r="C251" s="1" t="s">
         <v>527</v>
@@ -11053,7 +11062,7 @@
         <v>797</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>245</v>
+        <v>1606</v>
       </c>
       <c r="C252" s="1" t="s">
         <v>527</v>
@@ -11076,7 +11085,7 @@
         <v>798</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>246</v>
+        <v>1606</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>527</v>
@@ -11099,7 +11108,7 @@
         <v>799</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>247</v>
+        <v>1606</v>
       </c>
       <c r="C254" s="1" t="s">
         <v>527</v>
@@ -11122,7 +11131,7 @@
         <v>800</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>248</v>
+        <v>1606</v>
       </c>
       <c r="C255" s="1" t="s">
         <v>527</v>
@@ -11145,7 +11154,7 @@
         <v>801</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>249</v>
+        <v>1606</v>
       </c>
       <c r="C256" s="1" t="s">
         <v>527</v>
@@ -11168,7 +11177,7 @@
         <v>802</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>250</v>
+        <v>1606</v>
       </c>
       <c r="C257" s="1" t="s">
         <v>527</v>
@@ -11191,7 +11200,7 @@
         <v>803</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>251</v>
+        <v>1606</v>
       </c>
       <c r="C258" s="1" t="s">
         <v>527</v>
@@ -11214,7 +11223,7 @@
         <v>804</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>252</v>
+        <v>1606</v>
       </c>
       <c r="C259" s="1" t="s">
         <v>527</v>
@@ -11237,7 +11246,7 @@
         <v>805</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>253</v>
+        <v>1606</v>
       </c>
       <c r="C260" s="1" t="s">
         <v>527</v>
@@ -11260,7 +11269,7 @@
         <v>806</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>254</v>
+        <v>1606</v>
       </c>
       <c r="C261" s="1" t="s">
         <v>527</v>
@@ -11283,7 +11292,7 @@
         <v>807</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>255</v>
+        <v>1606</v>
       </c>
       <c r="C262" s="1" t="s">
         <v>527</v>
@@ -11306,7 +11315,7 @@
         <v>808</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>256</v>
+        <v>1606</v>
       </c>
       <c r="C263" s="1" t="s">
         <v>527</v>
@@ -11329,7 +11338,7 @@
         <v>809</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>257</v>
+        <v>1606</v>
       </c>
       <c r="C264" s="1" t="s">
         <v>527</v>
@@ -11352,7 +11361,7 @@
         <v>810</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>258</v>
+        <v>1606</v>
       </c>
       <c r="C265" s="1" t="s">
         <v>527</v>
@@ -11375,7 +11384,7 @@
         <v>811</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>259</v>
+        <v>1606</v>
       </c>
       <c r="C266" s="1" t="s">
         <v>527</v>
@@ -11398,7 +11407,7 @@
         <v>812</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>260</v>
+        <v>1606</v>
       </c>
       <c r="C267" s="1" t="s">
         <v>527</v>
@@ -11421,7 +11430,7 @@
         <v>813</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>261</v>
+        <v>1606</v>
       </c>
       <c r="C268" s="1" t="s">
         <v>527</v>
@@ -11444,7 +11453,7 @@
         <v>814</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>262</v>
+        <v>1606</v>
       </c>
       <c r="C269" s="1" t="s">
         <v>527</v>
@@ -11467,7 +11476,7 @@
         <v>815</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>263</v>
+        <v>1606</v>
       </c>
       <c r="C270" s="1" t="s">
         <v>527</v>
@@ -11490,7 +11499,7 @@
         <v>816</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>264</v>
+        <v>1606</v>
       </c>
       <c r="C271" s="1" t="s">
         <v>527</v>
@@ -11513,7 +11522,7 @@
         <v>817</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>265</v>
+        <v>1606</v>
       </c>
       <c r="C272" s="1" t="s">
         <v>527</v>
@@ -11536,7 +11545,7 @@
         <v>818</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>266</v>
+        <v>1606</v>
       </c>
       <c r="C273" s="1" t="s">
         <v>527</v>
@@ -11559,7 +11568,7 @@
         <v>819</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>267</v>
+        <v>1606</v>
       </c>
       <c r="C274" s="1" t="s">
         <v>527</v>
@@ -11582,7 +11591,7 @@
         <v>820</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>268</v>
+        <v>1606</v>
       </c>
       <c r="C275" s="1" t="s">
         <v>527</v>
@@ -11605,7 +11614,7 @@
         <v>821</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>269</v>
+        <v>1606</v>
       </c>
       <c r="C276" s="1" t="s">
         <v>527</v>
@@ -11628,7 +11637,7 @@
         <v>822</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>270</v>
+        <v>1606</v>
       </c>
       <c r="C277" s="1" t="s">
         <v>527</v>
@@ -11651,7 +11660,7 @@
         <v>823</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>271</v>
+        <v>1606</v>
       </c>
       <c r="C278" s="1" t="s">
         <v>527</v>
@@ -11674,7 +11683,7 @@
         <v>824</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>272</v>
+        <v>1606</v>
       </c>
       <c r="C279" s="1" t="s">
         <v>527</v>
@@ -11697,7 +11706,7 @@
         <v>825</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>273</v>
+        <v>1606</v>
       </c>
       <c r="C280" s="1" t="s">
         <v>527</v>
@@ -11720,7 +11729,7 @@
         <v>826</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>274</v>
+        <v>1606</v>
       </c>
       <c r="C281" s="1" t="s">
         <v>527</v>
@@ -11743,7 +11752,7 @@
         <v>827</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>275</v>
+        <v>1606</v>
       </c>
       <c r="C282" s="1" t="s">
         <v>527</v>
@@ -11766,7 +11775,7 @@
         <v>828</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>276</v>
+        <v>1606</v>
       </c>
       <c r="C283" s="1" t="s">
         <v>527</v>
@@ -11789,7 +11798,7 @@
         <v>829</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>277</v>
+        <v>1606</v>
       </c>
       <c r="C284" s="1" t="s">
         <v>527</v>
@@ -11812,7 +11821,7 @@
         <v>830</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>278</v>
+        <v>1606</v>
       </c>
       <c r="C285" s="1" t="s">
         <v>527</v>
@@ -11835,7 +11844,7 @@
         <v>831</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>279</v>
+        <v>1606</v>
       </c>
       <c r="C286" s="1" t="s">
         <v>527</v>
@@ -11858,7 +11867,7 @@
         <v>832</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>280</v>
+        <v>1606</v>
       </c>
       <c r="C287" s="1" t="s">
         <v>527</v>
@@ -11881,7 +11890,7 @@
         <v>833</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>281</v>
+        <v>1606</v>
       </c>
       <c r="C288" s="1" t="s">
         <v>527</v>
@@ -11904,7 +11913,7 @@
         <v>834</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>282</v>
+        <v>1606</v>
       </c>
       <c r="C289" s="1" t="s">
         <v>527</v>
@@ -11927,7 +11936,7 @@
         <v>835</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>283</v>
+        <v>1606</v>
       </c>
       <c r="C290" s="1" t="s">
         <v>527</v>
@@ -11950,7 +11959,7 @@
         <v>836</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>284</v>
+        <v>1606</v>
       </c>
       <c r="C291" s="1" t="s">
         <v>527</v>
@@ -11973,7 +11982,7 @@
         <v>837</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>285</v>
+        <v>1606</v>
       </c>
       <c r="C292" s="1" t="s">
         <v>527</v>
@@ -11996,7 +12005,7 @@
         <v>838</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>286</v>
+        <v>1606</v>
       </c>
       <c r="C293" s="1" t="s">
         <v>527</v>
@@ -12019,7 +12028,7 @@
         <v>839</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>287</v>
+        <v>1606</v>
       </c>
       <c r="C294" s="1" t="s">
         <v>527</v>
@@ -12042,7 +12051,7 @@
         <v>840</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>288</v>
+        <v>1606</v>
       </c>
       <c r="C295" s="1" t="s">
         <v>527</v>
@@ -12065,7 +12074,7 @@
         <v>841</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>289</v>
+        <v>1606</v>
       </c>
       <c r="C296" s="1" t="s">
         <v>527</v>
@@ -12088,7 +12097,7 @@
         <v>842</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>290</v>
+        <v>1606</v>
       </c>
       <c r="C297" s="1" t="s">
         <v>527</v>
@@ -12111,7 +12120,7 @@
         <v>843</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>291</v>
+        <v>1606</v>
       </c>
       <c r="C298" s="1" t="s">
         <v>527</v>
@@ -12134,7 +12143,7 @@
         <v>844</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>292</v>
+        <v>1606</v>
       </c>
       <c r="C299" s="1" t="s">
         <v>527</v>
@@ -12157,7 +12166,7 @@
         <v>845</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>293</v>
+        <v>1606</v>
       </c>
       <c r="C300" s="1" t="s">
         <v>527</v>
@@ -12180,7 +12189,7 @@
         <v>846</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>294</v>
+        <v>1606</v>
       </c>
       <c r="C301" s="1" t="s">
         <v>527</v>
@@ -12203,7 +12212,7 @@
         <v>847</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>295</v>
+        <v>1606</v>
       </c>
       <c r="C302" s="1" t="s">
         <v>527</v>
@@ -12226,7 +12235,7 @@
         <v>848</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>296</v>
+        <v>1606</v>
       </c>
       <c r="C303" s="1" t="s">
         <v>527</v>
@@ -12249,7 +12258,7 @@
         <v>849</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>297</v>
+        <v>1606</v>
       </c>
       <c r="C304" s="1" t="s">
         <v>527</v>
@@ -12272,7 +12281,7 @@
         <v>850</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>298</v>
+        <v>1606</v>
       </c>
       <c r="C305" s="1" t="s">
         <v>527</v>
@@ -12295,7 +12304,7 @@
         <v>851</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>299</v>
+        <v>1606</v>
       </c>
       <c r="C306" s="1" t="s">
         <v>527</v>
@@ -12318,7 +12327,7 @@
         <v>852</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>300</v>
+        <v>1606</v>
       </c>
       <c r="C307" s="1" t="s">
         <v>527</v>
@@ -12341,7 +12350,7 @@
         <v>853</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>7</v>
+        <v>1606</v>
       </c>
       <c r="C308" s="1" t="s">
         <v>527</v>
@@ -12364,7 +12373,7 @@
         <v>854</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>301</v>
+        <v>1606</v>
       </c>
       <c r="C309" s="1" t="s">
         <v>527</v>
@@ -12387,7 +12396,7 @@
         <v>855</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>302</v>
+        <v>1606</v>
       </c>
       <c r="C310" s="1" t="s">
         <v>527</v>
@@ -12410,7 +12419,7 @@
         <v>856</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>303</v>
+        <v>1606</v>
       </c>
       <c r="C311" s="1" t="s">
         <v>527</v>
@@ -12433,7 +12442,7 @@
         <v>857</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>304</v>
+        <v>1606</v>
       </c>
       <c r="C312" s="1" t="s">
         <v>527</v>
@@ -12456,7 +12465,7 @@
         <v>858</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>305</v>
+        <v>1606</v>
       </c>
       <c r="C313" s="1" t="s">
         <v>527</v>
@@ -12479,7 +12488,7 @@
         <v>859</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>306</v>
+        <v>1606</v>
       </c>
       <c r="C314" s="1" t="s">
         <v>527</v>
@@ -12502,7 +12511,7 @@
         <v>860</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>307</v>
+        <v>1606</v>
       </c>
       <c r="C315" s="1" t="s">
         <v>527</v>
@@ -12525,7 +12534,7 @@
         <v>861</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>308</v>
+        <v>1606</v>
       </c>
       <c r="C316" s="1" t="s">
         <v>527</v>
@@ -12548,7 +12557,7 @@
         <v>862</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>309</v>
+        <v>1606</v>
       </c>
       <c r="C317" s="1" t="s">
         <v>527</v>
@@ -12571,7 +12580,7 @@
         <v>863</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>310</v>
+        <v>1606</v>
       </c>
       <c r="C318" s="1" t="s">
         <v>527</v>
@@ -12594,7 +12603,7 @@
         <v>864</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>311</v>
+        <v>1606</v>
       </c>
       <c r="C319" s="1" t="s">
         <v>527</v>
@@ -12617,7 +12626,7 @@
         <v>865</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>312</v>
+        <v>1606</v>
       </c>
       <c r="C320" s="1" t="s">
         <v>527</v>
@@ -12640,7 +12649,7 @@
         <v>866</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>313</v>
+        <v>1606</v>
       </c>
       <c r="C321" s="1" t="s">
         <v>527</v>
@@ -12663,7 +12672,7 @@
         <v>867</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>12</v>
+        <v>1606</v>
       </c>
       <c r="C322" s="1" t="s">
         <v>527</v>
@@ -12686,7 +12695,7 @@
         <v>868</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>314</v>
+        <v>1606</v>
       </c>
       <c r="C323" s="1" t="s">
         <v>527</v>
@@ -12709,7 +12718,7 @@
         <v>869</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>315</v>
+        <v>1606</v>
       </c>
       <c r="C324" s="1" t="s">
         <v>527</v>
@@ -12732,7 +12741,7 @@
         <v>870</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>316</v>
+        <v>1606</v>
       </c>
       <c r="C325" s="1" t="s">
         <v>527</v>
@@ -12755,7 +12764,7 @@
         <v>871</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>317</v>
+        <v>1606</v>
       </c>
       <c r="C326" s="1" t="s">
         <v>527</v>
@@ -12778,7 +12787,7 @@
         <v>872</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>318</v>
+        <v>1606</v>
       </c>
       <c r="C327" s="1" t="s">
         <v>527</v>
@@ -12801,7 +12810,7 @@
         <v>873</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>319</v>
+        <v>1606</v>
       </c>
       <c r="C328" s="1" t="s">
         <v>527</v>
@@ -12824,7 +12833,7 @@
         <v>874</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>320</v>
+        <v>1606</v>
       </c>
       <c r="C329" s="1" t="s">
         <v>527</v>
@@ -12847,7 +12856,7 @@
         <v>875</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>321</v>
+        <v>1606</v>
       </c>
       <c r="C330" s="1" t="s">
         <v>527</v>
@@ -12870,7 +12879,7 @@
         <v>876</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>322</v>
+        <v>1606</v>
       </c>
       <c r="C331" s="1" t="s">
         <v>527</v>
@@ -12893,7 +12902,7 @@
         <v>877</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>323</v>
+        <v>1606</v>
       </c>
       <c r="C332" s="1" t="s">
         <v>527</v>
@@ -12916,7 +12925,7 @@
         <v>878</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>324</v>
+        <v>1606</v>
       </c>
       <c r="C333" s="1" t="s">
         <v>527</v>
@@ -12939,7 +12948,7 @@
         <v>879</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>325</v>
+        <v>1606</v>
       </c>
       <c r="C334" s="1" t="s">
         <v>527</v>
@@ -12962,7 +12971,7 @@
         <v>880</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>326</v>
+        <v>1606</v>
       </c>
       <c r="C335" s="1" t="s">
         <v>527</v>
@@ -12985,7 +12994,7 @@
         <v>881</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>327</v>
+        <v>1606</v>
       </c>
       <c r="C336" s="1" t="s">
         <v>527</v>
@@ -13008,7 +13017,7 @@
         <v>882</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>328</v>
+        <v>1606</v>
       </c>
       <c r="C337" s="1" t="s">
         <v>527</v>
@@ -13031,7 +13040,7 @@
         <v>883</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>329</v>
+        <v>1606</v>
       </c>
       <c r="C338" s="1" t="s">
         <v>527</v>
@@ -13054,7 +13063,7 @@
         <v>884</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>330</v>
+        <v>1606</v>
       </c>
       <c r="C339" s="1" t="s">
         <v>527</v>
@@ -13077,7 +13086,7 @@
         <v>885</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>331</v>
+        <v>1606</v>
       </c>
       <c r="C340" s="1" t="s">
         <v>527</v>
@@ -13100,7 +13109,7 @@
         <v>886</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>332</v>
+        <v>1606</v>
       </c>
       <c r="C341" s="1" t="s">
         <v>527</v>
@@ -13123,7 +13132,7 @@
         <v>887</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>333</v>
+        <v>1606</v>
       </c>
       <c r="C342" s="1" t="s">
         <v>527</v>
@@ -13146,7 +13155,7 @@
         <v>888</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>334</v>
+        <v>1606</v>
       </c>
       <c r="C343" s="1" t="s">
         <v>527</v>
@@ -13169,7 +13178,7 @@
         <v>889</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>335</v>
+        <v>1606</v>
       </c>
       <c r="C344" s="1" t="s">
         <v>527</v>
@@ -13192,7 +13201,7 @@
         <v>890</v>
       </c>
       <c r="B345" s="1" t="s">
-        <v>336</v>
+        <v>1606</v>
       </c>
       <c r="C345" s="1" t="s">
         <v>527</v>
@@ -13215,7 +13224,7 @@
         <v>891</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>337</v>
+        <v>1606</v>
       </c>
       <c r="C346" s="1" t="s">
         <v>527</v>
@@ -13238,7 +13247,7 @@
         <v>892</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>338</v>
+        <v>1606</v>
       </c>
       <c r="C347" s="1" t="s">
         <v>527</v>
@@ -13261,7 +13270,7 @@
         <v>893</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>339</v>
+        <v>1606</v>
       </c>
       <c r="C348" s="1" t="s">
         <v>527</v>
@@ -13284,7 +13293,7 @@
         <v>894</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>340</v>
+        <v>1606</v>
       </c>
       <c r="C349" s="1" t="s">
         <v>527</v>
@@ -13307,7 +13316,7 @@
         <v>895</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>341</v>
+        <v>1606</v>
       </c>
       <c r="C350" s="1" t="s">
         <v>527</v>
@@ -13330,7 +13339,7 @@
         <v>896</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>342</v>
+        <v>1606</v>
       </c>
       <c r="C351" s="1" t="s">
         <v>527</v>
@@ -13353,7 +13362,7 @@
         <v>897</v>
       </c>
       <c r="B352" s="1" t="s">
-        <v>343</v>
+        <v>1606</v>
       </c>
       <c r="C352" s="1" t="s">
         <v>527</v>
@@ -13376,7 +13385,7 @@
         <v>898</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>344</v>
+        <v>1606</v>
       </c>
       <c r="C353" s="1" t="s">
         <v>527</v>
@@ -13399,7 +13408,7 @@
         <v>899</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>345</v>
+        <v>1606</v>
       </c>
       <c r="C354" s="1" t="s">
         <v>527</v>
@@ -13422,7 +13431,7 @@
         <v>900</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>346</v>
+        <v>1606</v>
       </c>
       <c r="C355" s="1" t="s">
         <v>527</v>
@@ -13445,7 +13454,7 @@
         <v>901</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>347</v>
+        <v>1606</v>
       </c>
       <c r="C356" s="1" t="s">
         <v>527</v>
@@ -13468,7 +13477,7 @@
         <v>902</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>348</v>
+        <v>1606</v>
       </c>
       <c r="C357" s="1" t="s">
         <v>527</v>
@@ -13491,7 +13500,7 @@
         <v>903</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>349</v>
+        <v>1606</v>
       </c>
       <c r="C358" s="1" t="s">
         <v>527</v>
@@ -13514,7 +13523,7 @@
         <v>904</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>350</v>
+        <v>1606</v>
       </c>
       <c r="C359" s="1" t="s">
         <v>527</v>
@@ -13537,7 +13546,7 @@
         <v>905</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>310</v>
+        <v>1606</v>
       </c>
       <c r="C360" s="1" t="s">
         <v>527</v>
@@ -13560,7 +13569,7 @@
         <v>906</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>351</v>
+        <v>1606</v>
       </c>
       <c r="C361" s="1" t="s">
         <v>527</v>
@@ -13583,7 +13592,7 @@
         <v>907</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>352</v>
+        <v>1606</v>
       </c>
       <c r="C362" s="1" t="s">
         <v>527</v>
@@ -13606,7 +13615,7 @@
         <v>908</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>353</v>
+        <v>1606</v>
       </c>
       <c r="C363" s="1" t="s">
         <v>527</v>
@@ -13629,7 +13638,7 @@
         <v>909</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>354</v>
+        <v>1606</v>
       </c>
       <c r="C364" s="1" t="s">
         <v>527</v>
@@ -13652,7 +13661,7 @@
         <v>910</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>355</v>
+        <v>1606</v>
       </c>
       <c r="C365" s="1" t="s">
         <v>527</v>
@@ -13675,7 +13684,7 @@
         <v>911</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>356</v>
+        <v>1606</v>
       </c>
       <c r="C366" s="1" t="s">
         <v>527</v>
@@ -13698,7 +13707,7 @@
         <v>912</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>357</v>
+        <v>1606</v>
       </c>
       <c r="C367" s="1" t="s">
         <v>527</v>
@@ -13721,7 +13730,7 @@
         <v>913</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>358</v>
+        <v>1606</v>
       </c>
       <c r="C368" s="1" t="s">
         <v>527</v>
@@ -13744,7 +13753,7 @@
         <v>914</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>359</v>
+        <v>1606</v>
       </c>
       <c r="C369" s="1" t="s">
         <v>527</v>
@@ -13767,7 +13776,7 @@
         <v>915</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>360</v>
+        <v>1606</v>
       </c>
       <c r="C370" s="1" t="s">
         <v>527</v>
@@ -13790,7 +13799,7 @@
         <v>916</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>361</v>
+        <v>1606</v>
       </c>
       <c r="C371" s="1" t="s">
         <v>527</v>
@@ -13813,7 +13822,7 @@
         <v>917</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>362</v>
+        <v>1606</v>
       </c>
       <c r="C372" s="1" t="s">
         <v>527</v>
@@ -13836,7 +13845,7 @@
         <v>918</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>363</v>
+        <v>1606</v>
       </c>
       <c r="C373" s="1" t="s">
         <v>527</v>
@@ -13859,7 +13868,7 @@
         <v>919</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>364</v>
+        <v>1606</v>
       </c>
       <c r="C374" s="1" t="s">
         <v>527</v>
@@ -13882,7 +13891,7 @@
         <v>920</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>365</v>
+        <v>1606</v>
       </c>
       <c r="C375" s="1" t="s">
         <v>527</v>
@@ -13905,7 +13914,7 @@
         <v>921</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>366</v>
+        <v>1606</v>
       </c>
       <c r="C376" s="1" t="s">
         <v>527</v>
@@ -13928,7 +13937,7 @@
         <v>922</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>367</v>
+        <v>1606</v>
       </c>
       <c r="C377" s="1" t="s">
         <v>527</v>
@@ -13951,7 +13960,7 @@
         <v>923</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>368</v>
+        <v>1606</v>
       </c>
       <c r="C378" s="1" t="s">
         <v>527</v>
@@ -13974,7 +13983,7 @@
         <v>924</v>
       </c>
       <c r="B379" s="1" t="s">
-        <v>369</v>
+        <v>1606</v>
       </c>
       <c r="C379" s="1" t="s">
         <v>527</v>
@@ -13997,7 +14006,7 @@
         <v>925</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>370</v>
+        <v>1606</v>
       </c>
       <c r="C380" s="1" t="s">
         <v>527</v>
@@ -14020,7 +14029,7 @@
         <v>926</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>371</v>
+        <v>1606</v>
       </c>
       <c r="C381" s="1" t="s">
         <v>527</v>
@@ -14043,7 +14052,7 @@
         <v>927</v>
       </c>
       <c r="B382" s="1" t="s">
-        <v>372</v>
+        <v>1606</v>
       </c>
       <c r="C382" s="1" t="s">
         <v>527</v>
@@ -14066,7 +14075,7 @@
         <v>928</v>
       </c>
       <c r="B383" s="1" t="s">
-        <v>373</v>
+        <v>1606</v>
       </c>
       <c r="C383" s="1" t="s">
         <v>527</v>
@@ -14089,7 +14098,7 @@
         <v>929</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>374</v>
+        <v>1606</v>
       </c>
       <c r="C384" s="1" t="s">
         <v>527</v>
@@ -14112,7 +14121,7 @@
         <v>930</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>375</v>
+        <v>1606</v>
       </c>
       <c r="C385" s="1" t="s">
         <v>527</v>
@@ -14135,7 +14144,7 @@
         <v>931</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>342</v>
+        <v>1606</v>
       </c>
       <c r="C386" s="1" t="s">
         <v>527</v>
@@ -14158,7 +14167,7 @@
         <v>932</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>376</v>
+        <v>1606</v>
       </c>
       <c r="C387" s="1" t="s">
         <v>527</v>
@@ -14181,7 +14190,7 @@
         <v>933</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>377</v>
+        <v>1606</v>
       </c>
       <c r="C388" s="1" t="s">
         <v>527</v>
@@ -14204,7 +14213,7 @@
         <v>934</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>378</v>
+        <v>1606</v>
       </c>
       <c r="C389" s="1" t="s">
         <v>527</v>
@@ -14227,7 +14236,7 @@
         <v>935</v>
       </c>
       <c r="B390" s="1" t="s">
-        <v>379</v>
+        <v>1606</v>
       </c>
       <c r="C390" s="1" t="s">
         <v>527</v>
@@ -14250,7 +14259,7 @@
         <v>936</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>380</v>
+        <v>1606</v>
       </c>
       <c r="C391" s="1" t="s">
         <v>527</v>
@@ -14273,7 +14282,7 @@
         <v>937</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>381</v>
+        <v>1606</v>
       </c>
       <c r="C392" s="1" t="s">
         <v>527</v>
@@ -14296,7 +14305,7 @@
         <v>938</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>382</v>
+        <v>1606</v>
       </c>
       <c r="C393" s="1" t="s">
         <v>527</v>
@@ -14319,7 +14328,7 @@
         <v>939</v>
       </c>
       <c r="B394" s="1" t="s">
-        <v>383</v>
+        <v>1606</v>
       </c>
       <c r="C394" s="1" t="s">
         <v>527</v>
@@ -14342,7 +14351,7 @@
         <v>940</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>384</v>
+        <v>1606</v>
       </c>
       <c r="C395" s="1" t="s">
         <v>527</v>
@@ -14365,7 +14374,7 @@
         <v>941</v>
       </c>
       <c r="B396" s="1" t="s">
-        <v>385</v>
+        <v>1606</v>
       </c>
       <c r="C396" s="1" t="s">
         <v>527</v>
@@ -14388,7 +14397,7 @@
         <v>942</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>386</v>
+        <v>1606</v>
       </c>
       <c r="C397" s="1" t="s">
         <v>527</v>
@@ -14411,7 +14420,7 @@
         <v>943</v>
       </c>
       <c r="B398" s="1" t="s">
-        <v>387</v>
+        <v>1606</v>
       </c>
       <c r="C398" s="1" t="s">
         <v>527</v>
@@ -14434,7 +14443,7 @@
         <v>944</v>
       </c>
       <c r="B399" s="1" t="s">
-        <v>388</v>
+        <v>1606</v>
       </c>
       <c r="C399" s="1" t="s">
         <v>527</v>
@@ -14457,7 +14466,7 @@
         <v>945</v>
       </c>
       <c r="B400" s="1" t="s">
-        <v>389</v>
+        <v>1606</v>
       </c>
       <c r="C400" s="1" t="s">
         <v>527</v>
@@ -14480,7 +14489,7 @@
         <v>946</v>
       </c>
       <c r="B401" s="1" t="s">
-        <v>390</v>
+        <v>1606</v>
       </c>
       <c r="C401" s="1" t="s">
         <v>527</v>
@@ -14503,7 +14512,7 @@
         <v>947</v>
       </c>
       <c r="B402" s="1" t="s">
-        <v>391</v>
+        <v>1606</v>
       </c>
       <c r="C402" s="1" t="s">
         <v>527</v>
@@ -14526,7 +14535,7 @@
         <v>948</v>
       </c>
       <c r="B403" s="1" t="s">
-        <v>392</v>
+        <v>1606</v>
       </c>
       <c r="C403" s="1" t="s">
         <v>527</v>
@@ -14549,7 +14558,7 @@
         <v>949</v>
       </c>
       <c r="B404" s="1" t="s">
-        <v>393</v>
+        <v>1606</v>
       </c>
       <c r="C404" s="1" t="s">
         <v>527</v>
@@ -14572,7 +14581,7 @@
         <v>950</v>
       </c>
       <c r="B405" s="1" t="s">
-        <v>394</v>
+        <v>1606</v>
       </c>
       <c r="C405" s="1" t="s">
         <v>527</v>
@@ -14595,7 +14604,7 @@
         <v>951</v>
       </c>
       <c r="B406" s="1" t="s">
-        <v>395</v>
+        <v>1606</v>
       </c>
       <c r="C406" s="1" t="s">
         <v>527</v>
@@ -14618,7 +14627,7 @@
         <v>952</v>
       </c>
       <c r="B407" s="1" t="s">
-        <v>396</v>
+        <v>1606</v>
       </c>
       <c r="C407" s="1" t="s">
         <v>527</v>
@@ -14641,7 +14650,7 @@
         <v>953</v>
       </c>
       <c r="B408" s="1" t="s">
-        <v>397</v>
+        <v>1606</v>
       </c>
       <c r="C408" s="1" t="s">
         <v>527</v>
@@ -14664,7 +14673,7 @@
         <v>954</v>
       </c>
       <c r="B409" s="1" t="s">
-        <v>398</v>
+        <v>1606</v>
       </c>
       <c r="C409" s="1" t="s">
         <v>527</v>
@@ -14687,7 +14696,7 @@
         <v>955</v>
       </c>
       <c r="B410" s="1" t="s">
-        <v>399</v>
+        <v>1606</v>
       </c>
       <c r="C410" s="1" t="s">
         <v>527</v>
@@ -14710,7 +14719,7 @@
         <v>956</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>400</v>
+        <v>1606</v>
       </c>
       <c r="C411" s="1" t="s">
         <v>527</v>
@@ -14733,7 +14742,7 @@
         <v>957</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>401</v>
+        <v>1606</v>
       </c>
       <c r="C412" s="1" t="s">
         <v>527</v>
@@ -14756,7 +14765,7 @@
         <v>958</v>
       </c>
       <c r="B413" s="1" t="s">
-        <v>402</v>
+        <v>1606</v>
       </c>
       <c r="C413" s="1" t="s">
         <v>527</v>
@@ -14779,7 +14788,7 @@
         <v>959</v>
       </c>
       <c r="B414" s="1" t="s">
-        <v>403</v>
+        <v>1606</v>
       </c>
       <c r="C414" s="1" t="s">
         <v>527</v>
@@ -14802,7 +14811,7 @@
         <v>960</v>
       </c>
       <c r="B415" s="1" t="s">
-        <v>404</v>
+        <v>1606</v>
       </c>
       <c r="C415" s="1" t="s">
         <v>527</v>
@@ -14825,7 +14834,7 @@
         <v>961</v>
       </c>
       <c r="B416" s="1" t="s">
-        <v>405</v>
+        <v>1606</v>
       </c>
       <c r="C416" s="1" t="s">
         <v>527</v>
@@ -14848,7 +14857,7 @@
         <v>962</v>
       </c>
       <c r="B417" s="1" t="s">
-        <v>406</v>
+        <v>1606</v>
       </c>
       <c r="C417" s="1" t="s">
         <v>527</v>
@@ -14871,7 +14880,7 @@
         <v>963</v>
       </c>
       <c r="B418" s="1" t="s">
-        <v>407</v>
+        <v>1606</v>
       </c>
       <c r="C418" s="1" t="s">
         <v>527</v>
@@ -14894,7 +14903,7 @@
         <v>964</v>
       </c>
       <c r="B419" s="1" t="s">
-        <v>408</v>
+        <v>1606</v>
       </c>
       <c r="C419" s="1" t="s">
         <v>527</v>
@@ -14917,7 +14926,7 @@
         <v>965</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>409</v>
+        <v>1606</v>
       </c>
       <c r="C420" s="1" t="s">
         <v>527</v>
@@ -14940,7 +14949,7 @@
         <v>966</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>410</v>
+        <v>1606</v>
       </c>
       <c r="C421" s="1" t="s">
         <v>527</v>
@@ -14963,7 +14972,7 @@
         <v>967</v>
       </c>
       <c r="B422" s="1" t="s">
-        <v>411</v>
+        <v>1606</v>
       </c>
       <c r="C422" s="1" t="s">
         <v>527</v>
@@ -14986,7 +14995,7 @@
         <v>968</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>412</v>
+        <v>1606</v>
       </c>
       <c r="C423" s="1" t="s">
         <v>527</v>
@@ -15009,7 +15018,7 @@
         <v>969</v>
       </c>
       <c r="B424" s="1" t="s">
-        <v>413</v>
+        <v>1606</v>
       </c>
       <c r="C424" s="1" t="s">
         <v>527</v>
@@ -15032,7 +15041,7 @@
         <v>970</v>
       </c>
       <c r="B425" s="1" t="s">
-        <v>414</v>
+        <v>1606</v>
       </c>
       <c r="C425" s="1" t="s">
         <v>527</v>
@@ -15055,7 +15064,7 @@
         <v>971</v>
       </c>
       <c r="B426" s="1" t="s">
-        <v>415</v>
+        <v>1606</v>
       </c>
       <c r="C426" s="1" t="s">
         <v>527</v>
@@ -15078,7 +15087,7 @@
         <v>972</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>416</v>
+        <v>1606</v>
       </c>
       <c r="C427" s="1" t="s">
         <v>527</v>
@@ -15101,7 +15110,7 @@
         <v>973</v>
       </c>
       <c r="B428" s="1" t="s">
-        <v>417</v>
+        <v>1606</v>
       </c>
       <c r="C428" s="1" t="s">
         <v>527</v>
@@ -15124,7 +15133,7 @@
         <v>974</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>418</v>
+        <v>1606</v>
       </c>
       <c r="C429" s="1" t="s">
         <v>527</v>
@@ -15147,7 +15156,7 @@
         <v>975</v>
       </c>
       <c r="B430" s="1" t="s">
-        <v>419</v>
+        <v>1606</v>
       </c>
       <c r="C430" s="1" t="s">
         <v>527</v>
@@ -15170,7 +15179,7 @@
         <v>976</v>
       </c>
       <c r="B431" s="1" t="s">
-        <v>420</v>
+        <v>1606</v>
       </c>
       <c r="C431" s="1" t="s">
         <v>527</v>
@@ -15193,7 +15202,7 @@
         <v>977</v>
       </c>
       <c r="B432" s="1" t="s">
-        <v>421</v>
+        <v>1606</v>
       </c>
       <c r="C432" s="1" t="s">
         <v>527</v>
@@ -15216,7 +15225,7 @@
         <v>978</v>
       </c>
       <c r="B433" s="1" t="s">
-        <v>422</v>
+        <v>1606</v>
       </c>
       <c r="C433" s="1" t="s">
         <v>527</v>
@@ -15239,7 +15248,7 @@
         <v>979</v>
       </c>
       <c r="B434" s="1" t="s">
-        <v>423</v>
+        <v>1606</v>
       </c>
       <c r="C434" s="1" t="s">
         <v>527</v>
@@ -15262,7 +15271,7 @@
         <v>980</v>
       </c>
       <c r="B435" s="1" t="s">
-        <v>424</v>
+        <v>1606</v>
       </c>
       <c r="C435" s="1" t="s">
         <v>527</v>
@@ -15285,7 +15294,7 @@
         <v>981</v>
       </c>
       <c r="B436" s="1" t="s">
-        <v>425</v>
+        <v>1606</v>
       </c>
       <c r="C436" s="1" t="s">
         <v>527</v>
@@ -15308,7 +15317,7 @@
         <v>982</v>
       </c>
       <c r="B437" s="1" t="s">
-        <v>426</v>
+        <v>1606</v>
       </c>
       <c r="C437" s="1" t="s">
         <v>527</v>
@@ -15331,7 +15340,7 @@
         <v>983</v>
       </c>
       <c r="B438" s="1" t="s">
-        <v>427</v>
+        <v>1606</v>
       </c>
       <c r="C438" s="1" t="s">
         <v>527</v>
@@ -15354,7 +15363,7 @@
         <v>984</v>
       </c>
       <c r="B439" s="1" t="s">
-        <v>428</v>
+        <v>1606</v>
       </c>
       <c r="C439" s="1" t="s">
         <v>527</v>
@@ -15377,7 +15386,7 @@
         <v>985</v>
       </c>
       <c r="B440" s="1" t="s">
-        <v>429</v>
+        <v>1606</v>
       </c>
       <c r="C440" s="1" t="s">
         <v>527</v>
@@ -15400,7 +15409,7 @@
         <v>986</v>
       </c>
       <c r="B441" s="1" t="s">
-        <v>430</v>
+        <v>1606</v>
       </c>
       <c r="C441" s="1" t="s">
         <v>527</v>
@@ -15423,7 +15432,7 @@
         <v>987</v>
       </c>
       <c r="B442" s="1" t="s">
-        <v>431</v>
+        <v>1606</v>
       </c>
       <c r="C442" s="1" t="s">
         <v>527</v>
@@ -15446,7 +15455,7 @@
         <v>988</v>
       </c>
       <c r="B443" s="1" t="s">
-        <v>432</v>
+        <v>1606</v>
       </c>
       <c r="C443" s="1" t="s">
         <v>527</v>
@@ -15469,7 +15478,7 @@
         <v>989</v>
       </c>
       <c r="B444" s="1" t="s">
-        <v>433</v>
+        <v>1606</v>
       </c>
       <c r="C444" s="1" t="s">
         <v>527</v>
@@ -15492,7 +15501,7 @@
         <v>990</v>
       </c>
       <c r="B445" s="1" t="s">
-        <v>434</v>
+        <v>1606</v>
       </c>
       <c r="C445" s="1" t="s">
         <v>527</v>
@@ -15515,7 +15524,7 @@
         <v>991</v>
       </c>
       <c r="B446" s="1" t="s">
-        <v>435</v>
+        <v>1606</v>
       </c>
       <c r="C446" s="1" t="s">
         <v>527</v>
@@ -15538,7 +15547,7 @@
         <v>992</v>
       </c>
       <c r="B447" s="1" t="s">
-        <v>436</v>
+        <v>1606</v>
       </c>
       <c r="C447" s="1" t="s">
         <v>527</v>
@@ -15561,7 +15570,7 @@
         <v>993</v>
       </c>
       <c r="B448" s="1" t="s">
-        <v>437</v>
+        <v>1606</v>
       </c>
       <c r="C448" s="1" t="s">
         <v>527</v>
@@ -15584,7 +15593,7 @@
         <v>994</v>
       </c>
       <c r="B449" s="1" t="s">
-        <v>438</v>
+        <v>1606</v>
       </c>
       <c r="C449" s="1" t="s">
         <v>527</v>
@@ -15607,7 +15616,7 @@
         <v>995</v>
       </c>
       <c r="B450" s="1" t="s">
-        <v>439</v>
+        <v>1606</v>
       </c>
       <c r="C450" s="1" t="s">
         <v>527</v>
@@ -15630,7 +15639,7 @@
         <v>996</v>
       </c>
       <c r="B451" s="1" t="s">
-        <v>440</v>
+        <v>1606</v>
       </c>
       <c r="C451" s="1" t="s">
         <v>527</v>
@@ -15653,7 +15662,7 @@
         <v>997</v>
       </c>
       <c r="B452" s="1" t="s">
-        <v>441</v>
+        <v>1606</v>
       </c>
       <c r="C452" s="1" t="s">
         <v>527</v>
@@ -15676,7 +15685,7 @@
         <v>998</v>
       </c>
       <c r="B453" s="1" t="s">
-        <v>442</v>
+        <v>1606</v>
       </c>
       <c r="C453" s="1" t="s">
         <v>527</v>
@@ -15699,7 +15708,7 @@
         <v>999</v>
       </c>
       <c r="B454" s="1" t="s">
-        <v>443</v>
+        <v>1606</v>
       </c>
       <c r="C454" s="1" t="s">
         <v>527</v>
@@ -15722,7 +15731,7 @@
         <v>1000</v>
       </c>
       <c r="B455" s="1" t="s">
-        <v>444</v>
+        <v>1606</v>
       </c>
       <c r="C455" s="1" t="s">
         <v>527</v>
@@ -15745,7 +15754,7 @@
         <v>1001</v>
       </c>
       <c r="B456" s="1" t="s">
-        <v>445</v>
+        <v>1606</v>
       </c>
       <c r="C456" s="1" t="s">
         <v>527</v>
@@ -15768,7 +15777,7 @@
         <v>1002</v>
       </c>
       <c r="B457" s="1" t="s">
-        <v>446</v>
+        <v>1606</v>
       </c>
       <c r="C457" s="1" t="s">
         <v>527</v>
@@ -15791,7 +15800,7 @@
         <v>1003</v>
       </c>
       <c r="B458" s="1" t="s">
-        <v>447</v>
+        <v>1606</v>
       </c>
       <c r="C458" s="1" t="s">
         <v>527</v>
@@ -15814,7 +15823,7 @@
         <v>1004</v>
       </c>
       <c r="B459" s="1" t="s">
-        <v>448</v>
+        <v>1606</v>
       </c>
       <c r="C459" s="1" t="s">
         <v>527</v>
@@ -15837,7 +15846,7 @@
         <v>1005</v>
       </c>
       <c r="B460" s="1" t="s">
-        <v>449</v>
+        <v>1606</v>
       </c>
       <c r="C460" s="1" t="s">
         <v>527</v>
@@ -15860,7 +15869,7 @@
         <v>1006</v>
       </c>
       <c r="B461" s="1" t="s">
-        <v>450</v>
+        <v>1606</v>
       </c>
       <c r="C461" s="1" t="s">
         <v>527</v>
@@ -15883,7 +15892,7 @@
         <v>1007</v>
       </c>
       <c r="B462" s="1" t="s">
-        <v>451</v>
+        <v>1606</v>
       </c>
       <c r="C462" s="1" t="s">
         <v>527</v>
@@ -15906,7 +15915,7 @@
         <v>1008</v>
       </c>
       <c r="B463" s="1" t="s">
-        <v>452</v>
+        <v>1606</v>
       </c>
       <c r="C463" s="1" t="s">
         <v>527</v>
@@ -15929,7 +15938,7 @@
         <v>1009</v>
       </c>
       <c r="B464" s="1" t="s">
-        <v>453</v>
+        <v>1606</v>
       </c>
       <c r="C464" s="1" t="s">
         <v>527</v>
@@ -15952,7 +15961,7 @@
         <v>1010</v>
       </c>
       <c r="B465" s="1" t="s">
-        <v>454</v>
+        <v>1606</v>
       </c>
       <c r="C465" s="1" t="s">
         <v>527</v>
@@ -15975,7 +15984,7 @@
         <v>1011</v>
       </c>
       <c r="B466" s="1" t="s">
-        <v>455</v>
+        <v>1606</v>
       </c>
       <c r="C466" s="1" t="s">
         <v>527</v>
@@ -15998,7 +16007,7 @@
         <v>1012</v>
       </c>
       <c r="B467" s="1" t="s">
-        <v>456</v>
+        <v>1606</v>
       </c>
       <c r="C467" s="1" t="s">
         <v>527</v>
@@ -16021,7 +16030,7 @@
         <v>1013</v>
       </c>
       <c r="B468" s="1" t="s">
-        <v>457</v>
+        <v>1606</v>
       </c>
       <c r="C468" s="1" t="s">
         <v>527</v>
@@ -16044,7 +16053,7 @@
         <v>1014</v>
       </c>
       <c r="B469" s="1" t="s">
-        <v>458</v>
+        <v>1606</v>
       </c>
       <c r="C469" s="1" t="s">
         <v>527</v>
@@ -16067,7 +16076,7 @@
         <v>1015</v>
       </c>
       <c r="B470" s="1" t="s">
-        <v>459</v>
+        <v>1606</v>
       </c>
       <c r="C470" s="1" t="s">
         <v>527</v>
@@ -16090,7 +16099,7 @@
         <v>1016</v>
       </c>
       <c r="B471" s="1" t="s">
-        <v>460</v>
+        <v>1606</v>
       </c>
       <c r="C471" s="1" t="s">
         <v>527</v>
@@ -16113,7 +16122,7 @@
         <v>1017</v>
       </c>
       <c r="B472" s="1" t="s">
-        <v>461</v>
+        <v>1606</v>
       </c>
       <c r="C472" s="1" t="s">
         <v>527</v>
@@ -16136,7 +16145,7 @@
         <v>1018</v>
       </c>
       <c r="B473" s="1" t="s">
-        <v>314</v>
+        <v>1606</v>
       </c>
       <c r="C473" s="1" t="s">
         <v>527</v>
@@ -16159,7 +16168,7 @@
         <v>1019</v>
       </c>
       <c r="B474" s="1" t="s">
-        <v>462</v>
+        <v>1606</v>
       </c>
       <c r="C474" s="1" t="s">
         <v>546</v>
@@ -16182,7 +16191,7 @@
         <v>1020</v>
       </c>
       <c r="B475" s="1" t="s">
-        <v>463</v>
+        <v>1606</v>
       </c>
       <c r="C475" s="1" t="s">
         <v>546</v>
@@ -16205,7 +16214,7 @@
         <v>1021</v>
       </c>
       <c r="B476" s="1" t="s">
-        <v>464</v>
+        <v>1606</v>
       </c>
       <c r="C476" s="1" t="s">
         <v>546</v>
@@ -16228,7 +16237,7 @@
         <v>1022</v>
       </c>
       <c r="B477" s="1" t="s">
-        <v>465</v>
+        <v>1606</v>
       </c>
       <c r="C477" s="1" t="s">
         <v>546</v>
@@ -16251,7 +16260,7 @@
         <v>1023</v>
       </c>
       <c r="B478" s="1" t="s">
-        <v>466</v>
+        <v>1606</v>
       </c>
       <c r="C478" s="1" t="s">
         <v>546</v>
@@ -16274,7 +16283,7 @@
         <v>1024</v>
       </c>
       <c r="B479" s="1" t="s">
-        <v>467</v>
+        <v>1606</v>
       </c>
       <c r="C479" s="1" t="s">
         <v>546</v>
@@ -16297,7 +16306,7 @@
         <v>1025</v>
       </c>
       <c r="B480" s="1" t="s">
-        <v>468</v>
+        <v>1606</v>
       </c>
       <c r="C480" s="1" t="s">
         <v>546</v>
@@ -16320,7 +16329,7 @@
         <v>1026</v>
       </c>
       <c r="B481" s="1" t="s">
-        <v>469</v>
+        <v>1606</v>
       </c>
       <c r="C481" s="1" t="s">
         <v>546</v>
@@ -16343,7 +16352,7 @@
         <v>1027</v>
       </c>
       <c r="B482" s="1" t="s">
-        <v>470</v>
+        <v>1606</v>
       </c>
       <c r="C482" s="1" t="s">
         <v>546</v>
@@ -16366,7 +16375,7 @@
         <v>1028</v>
       </c>
       <c r="B483" s="1" t="s">
-        <v>471</v>
+        <v>1606</v>
       </c>
       <c r="C483" s="1" t="s">
         <v>546</v>
@@ -16389,7 +16398,7 @@
         <v>1029</v>
       </c>
       <c r="B484" s="1" t="s">
-        <v>472</v>
+        <v>1606</v>
       </c>
       <c r="C484" s="1" t="s">
         <v>546</v>
@@ -16412,7 +16421,7 @@
         <v>1030</v>
       </c>
       <c r="B485" s="1" t="s">
-        <v>438</v>
+        <v>1606</v>
       </c>
       <c r="C485" s="1" t="s">
         <v>546</v>
@@ -16435,7 +16444,7 @@
         <v>1031</v>
       </c>
       <c r="B486" s="1" t="s">
-        <v>473</v>
+        <v>1606</v>
       </c>
       <c r="C486" s="1" t="s">
         <v>546</v>
@@ -16458,7 +16467,7 @@
         <v>1032</v>
       </c>
       <c r="B487" s="1" t="s">
-        <v>474</v>
+        <v>1606</v>
       </c>
       <c r="C487" s="1" t="s">
         <v>546</v>
@@ -16481,7 +16490,7 @@
         <v>1033</v>
       </c>
       <c r="B488" s="1" t="s">
-        <v>475</v>
+        <v>1606</v>
       </c>
       <c r="C488" s="1" t="s">
         <v>546</v>
@@ -16504,7 +16513,7 @@
         <v>1034</v>
       </c>
       <c r="B489" s="1" t="s">
-        <v>476</v>
+        <v>1606</v>
       </c>
       <c r="C489" s="1" t="s">
         <v>546</v>
@@ -16527,7 +16536,7 @@
         <v>1035</v>
       </c>
       <c r="B490" s="1" t="s">
-        <v>477</v>
+        <v>1606</v>
       </c>
       <c r="C490" s="1" t="s">
         <v>546</v>
@@ -16550,7 +16559,7 @@
         <v>1036</v>
       </c>
       <c r="B491" s="1" t="s">
-        <v>478</v>
+        <v>1606</v>
       </c>
       <c r="C491" s="1" t="s">
         <v>546</v>
@@ -16573,7 +16582,7 @@
         <v>1037</v>
       </c>
       <c r="B492" s="1" t="s">
-        <v>479</v>
+        <v>1606</v>
       </c>
       <c r="C492" s="1" t="s">
         <v>546</v>
@@ -16596,7 +16605,7 @@
         <v>1038</v>
       </c>
       <c r="B493" s="1" t="s">
-        <v>97</v>
+        <v>1606</v>
       </c>
       <c r="C493" s="1" t="s">
         <v>546</v>
@@ -16619,7 +16628,7 @@
         <v>1039</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>480</v>
+        <v>1606</v>
       </c>
       <c r="C494" s="1" t="s">
         <v>546</v>
@@ -16642,7 +16651,7 @@
         <v>1040</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>481</v>
+        <v>1606</v>
       </c>
       <c r="C495" s="1" t="s">
         <v>546</v>
@@ -16665,7 +16674,7 @@
         <v>1041</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>482</v>
+        <v>1606</v>
       </c>
       <c r="C496" s="1" t="s">
         <v>546</v>
@@ -16688,7 +16697,7 @@
         <v>1042</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>483</v>
+        <v>1606</v>
       </c>
       <c r="C497" s="1" t="s">
         <v>546</v>
@@ -16711,7 +16720,7 @@
         <v>1043</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>484</v>
+        <v>1606</v>
       </c>
       <c r="C498" s="1" t="s">
         <v>546</v>
@@ -16734,7 +16743,7 @@
         <v>1044</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>318</v>
+        <v>1606</v>
       </c>
       <c r="C499" s="1" t="s">
         <v>546</v>
@@ -16757,7 +16766,7 @@
         <v>1045</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>379</v>
+        <v>1606</v>
       </c>
       <c r="C500" s="1" t="s">
         <v>546</v>
@@ -16780,7 +16789,7 @@
         <v>1046</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>485</v>
+        <v>1606</v>
       </c>
       <c r="C501" s="1" t="s">
         <v>546</v>
@@ -16803,7 +16812,7 @@
         <v>1047</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>486</v>
+        <v>1606</v>
       </c>
       <c r="C502" s="1" t="s">
         <v>546</v>
@@ -16826,7 +16835,7 @@
         <v>1048</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>487</v>
+        <v>1606</v>
       </c>
       <c r="C503" s="1" t="s">
         <v>546</v>
@@ -16849,7 +16858,7 @@
         <v>1049</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>488</v>
+        <v>1606</v>
       </c>
       <c r="C504" s="1" t="s">
         <v>546</v>
@@ -16872,7 +16881,7 @@
         <v>1050</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>489</v>
+        <v>1606</v>
       </c>
       <c r="C505" s="1" t="s">
         <v>546</v>
@@ -16895,7 +16904,7 @@
         <v>1051</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>490</v>
+        <v>1606</v>
       </c>
       <c r="C506" s="1" t="s">
         <v>546</v>
@@ -16918,7 +16927,7 @@
         <v>1052</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>491</v>
+        <v>1606</v>
       </c>
       <c r="C507" s="1" t="s">
         <v>546</v>
@@ -16941,7 +16950,7 @@
         <v>1053</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>492</v>
+        <v>1606</v>
       </c>
       <c r="C508" s="1" t="s">
         <v>546</v>
@@ -16964,7 +16973,7 @@
         <v>1054</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>493</v>
+        <v>1606</v>
       </c>
       <c r="C509" s="1" t="s">
         <v>546</v>
@@ -16987,7 +16996,7 @@
         <v>1055</v>
       </c>
       <c r="B510" s="1" t="s">
-        <v>494</v>
+        <v>1606</v>
       </c>
       <c r="C510" s="1" t="s">
         <v>546</v>
@@ -17010,7 +17019,7 @@
         <v>1056</v>
       </c>
       <c r="B511" s="1" t="s">
-        <v>495</v>
+        <v>1606</v>
       </c>
       <c r="C511" s="1" t="s">
         <v>546</v>
@@ -17033,7 +17042,7 @@
         <v>1057</v>
       </c>
       <c r="B512" s="1" t="s">
-        <v>352</v>
+        <v>1606</v>
       </c>
       <c r="C512" s="1" t="s">
         <v>546</v>
@@ -17056,7 +17065,7 @@
         <v>1058</v>
       </c>
       <c r="B513" s="1" t="s">
-        <v>345</v>
+        <v>1606</v>
       </c>
       <c r="C513" s="1" t="s">
         <v>546</v>
@@ -17079,7 +17088,7 @@
         <v>1059</v>
       </c>
       <c r="B514" s="1" t="s">
-        <v>238</v>
+        <v>1606</v>
       </c>
       <c r="C514" s="1" t="s">
         <v>546</v>
@@ -17102,7 +17111,7 @@
         <v>1060</v>
       </c>
       <c r="B515" s="1" t="s">
-        <v>496</v>
+        <v>1606</v>
       </c>
       <c r="C515" s="1" t="s">
         <v>546</v>
@@ -17125,7 +17134,7 @@
         <v>1061</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>497</v>
+        <v>1606</v>
       </c>
       <c r="C516" s="1" t="s">
         <v>546</v>
@@ -17148,7 +17157,7 @@
         <v>1062</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>498</v>
+        <v>1606</v>
       </c>
       <c r="C517" s="1" t="s">
         <v>546</v>
@@ -17171,7 +17180,7 @@
         <v>1063</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>499</v>
+        <v>1606</v>
       </c>
       <c r="C518" s="1" t="s">
         <v>546</v>
@@ -17194,7 +17203,7 @@
         <v>1064</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>236</v>
+        <v>1606</v>
       </c>
       <c r="C519" s="1" t="s">
         <v>546</v>
@@ -17217,7 +17226,7 @@
         <v>1065</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>500</v>
+        <v>1606</v>
       </c>
       <c r="C520" s="1" t="s">
         <v>546</v>
@@ -17240,7 +17249,7 @@
         <v>1066</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>501</v>
+        <v>1606</v>
       </c>
       <c r="C521" s="1" t="s">
         <v>546</v>
@@ -17263,7 +17272,7 @@
         <v>1067</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>502</v>
+        <v>1606</v>
       </c>
       <c r="C522" s="1" t="s">
         <v>546</v>
@@ -17286,7 +17295,7 @@
         <v>1068</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>503</v>
+        <v>1606</v>
       </c>
       <c r="C523" s="1" t="s">
         <v>546</v>
@@ -17309,7 +17318,7 @@
         <v>1069</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>504</v>
+        <v>1606</v>
       </c>
       <c r="C524" s="1" t="s">
         <v>546</v>
@@ -17332,7 +17341,7 @@
         <v>1070</v>
       </c>
       <c r="B525" s="1" t="s">
-        <v>505</v>
+        <v>1606</v>
       </c>
       <c r="C525" s="1" t="s">
         <v>546</v>
@@ -17355,7 +17364,7 @@
         <v>1071</v>
       </c>
       <c r="B526" s="1" t="s">
-        <v>304</v>
+        <v>1606</v>
       </c>
       <c r="C526" s="1" t="s">
         <v>546</v>
@@ -17378,7 +17387,7 @@
         <v>1072</v>
       </c>
       <c r="B527" s="1" t="s">
-        <v>506</v>
+        <v>1606</v>
       </c>
       <c r="C527" s="1" t="s">
         <v>546</v>
@@ -17401,7 +17410,7 @@
         <v>1073</v>
       </c>
       <c r="B528" s="1" t="s">
-        <v>507</v>
+        <v>1606</v>
       </c>
       <c r="C528" s="1" t="s">
         <v>546</v>
@@ -17424,7 +17433,7 @@
         <v>1074</v>
       </c>
       <c r="B529" s="1" t="s">
-        <v>508</v>
+        <v>1606</v>
       </c>
       <c r="C529" s="1" t="s">
         <v>546</v>
@@ -17447,7 +17456,7 @@
         <v>1075</v>
       </c>
       <c r="B530" s="1" t="s">
-        <v>509</v>
+        <v>1606</v>
       </c>
       <c r="C530" s="1" t="s">
         <v>546</v>
@@ -17469,7 +17478,9 @@
       <c r="A531" s="1" t="s">
         <v>1076</v>
       </c>
-      <c r="B531" s="1"/>
+      <c r="B531" s="1" t="s">
+        <v>1606</v>
+      </c>
       <c r="C531" s="1" t="s">
         <v>546</v>
       </c>
@@ -17486,7 +17497,7 @@
         <v>1077</v>
       </c>
       <c r="B532" s="1" t="s">
-        <v>496</v>
+        <v>1606</v>
       </c>
       <c r="C532" s="1" t="s">
         <v>546</v>
@@ -17509,7 +17520,7 @@
         <v>1078</v>
       </c>
       <c r="B533" s="1" t="s">
-        <v>510</v>
+        <v>1606</v>
       </c>
       <c r="C533" s="1" t="s">
         <v>546</v>
@@ -17532,7 +17543,7 @@
         <v>1079</v>
       </c>
       <c r="B534" s="1" t="s">
-        <v>511</v>
+        <v>1606</v>
       </c>
       <c r="C534" s="1" t="s">
         <v>546</v>
@@ -17555,7 +17566,7 @@
         <v>1080</v>
       </c>
       <c r="B535" s="1" t="s">
-        <v>512</v>
+        <v>1606</v>
       </c>
       <c r="C535" s="1" t="s">
         <v>546</v>
@@ -17578,7 +17589,7 @@
         <v>1081</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>513</v>
+        <v>1606</v>
       </c>
       <c r="C536" s="1" t="s">
         <v>546</v>
@@ -17601,7 +17612,7 @@
         <v>1082</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>514</v>
+        <v>1606</v>
       </c>
       <c r="C537" s="1" t="s">
         <v>546</v>
@@ -17624,7 +17635,7 @@
         <v>1083</v>
       </c>
       <c r="B538" s="1" t="s">
-        <v>161</v>
+        <v>1606</v>
       </c>
       <c r="C538" s="1" t="s">
         <v>546</v>
@@ -17647,7 +17658,7 @@
         <v>1084</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>222</v>
+        <v>1606</v>
       </c>
       <c r="C539" s="1" t="s">
         <v>546</v>
@@ -17670,7 +17681,7 @@
         <v>1085</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>515</v>
+        <v>1606</v>
       </c>
       <c r="C540" s="1" t="s">
         <v>546</v>
@@ -17693,7 +17704,7 @@
         <v>1086</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>88</v>
+        <v>1606</v>
       </c>
       <c r="C541" s="1" t="s">
         <v>546</v>
@@ -17716,7 +17727,7 @@
         <v>1087</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>516</v>
+        <v>1606</v>
       </c>
       <c r="C542" s="1" t="s">
         <v>546</v>
@@ -17739,7 +17750,7 @@
         <v>1088</v>
       </c>
       <c r="B543" s="1" t="s">
-        <v>517</v>
+        <v>1606</v>
       </c>
       <c r="C543" s="1" t="s">
         <v>546</v>
@@ -17762,7 +17773,7 @@
         <v>1089</v>
       </c>
       <c r="B544" s="1" t="s">
-        <v>513</v>
+        <v>1606</v>
       </c>
       <c r="C544" s="1" t="s">
         <v>546</v>

</xml_diff>